<commit_message>
added slide on streams
</commit_message>
<xml_diff>
--- a/UFS 05 - Programmazione in Java e strumenti per lo sviluppo/voti_es_swing-disegno oggetti con timers.xlsx
+++ b/UFS 05 - Programmazione in Java e strumenti per lo sviluppo/voti_es_swing-disegno oggetti con timers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ingconti/Documents/GIT/its_rizzoli/UFS 05 - Programmazione in Java e strumenti per lo sviluppo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{685BA25C-01E4-6442-916F-E010FBEA7AD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E16DC58-6572-454F-BDE6-8408387466EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2780" yWindow="1500" windowWidth="28040" windowHeight="17440" xr2:uid="{2EDEC0AA-C08D-1046-93D2-E53883CA382D}"/>
+    <workbookView xWindow="340" yWindow="760" windowWidth="29820" windowHeight="19240" xr2:uid="{2EDEC0AA-C08D-1046-93D2-E53883CA382D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="40">
   <si>
     <t>Nome Studente</t>
   </si>
@@ -76,9 +76,6 @@
     <t>Hanu Cristian</t>
   </si>
   <si>
-    <t>Hanu Robert</t>
-  </si>
-  <si>
     <t>Lin Chen Wei Riccardo</t>
   </si>
   <si>
@@ -112,7 +109,52 @@
     <t>Zulini Gabriele</t>
   </si>
   <si>
-    <t>oggetti grafici swing</t>
+    <t>note</t>
+  </si>
+  <si>
+    <t>LAVORO X CASA</t>
+  </si>
+  <si>
+    <t>oggetti grafici swing Phase2</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>assente</t>
+  </si>
+  <si>
+    <t>ok</t>
+  </si>
+  <si>
+    <t>posizioni fisse - non scala le posizioni - veirifcare JPGE</t>
+  </si>
+  <si>
+    <t>nc</t>
+  </si>
+  <si>
+    <t>exception - dimensioni  fisse</t>
+  </si>
+  <si>
+    <t>incompleto</t>
+  </si>
+  <si>
+    <t>manca</t>
+  </si>
+  <si>
+    <t>cancellata</t>
+  </si>
+  <si>
+    <t>ok, manca zoom manca timers</t>
+  </si>
+  <si>
+    <t>--</t>
+  </si>
+  <si>
+    <t>non si trova project intelliJ</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> --</t>
   </si>
 </sst>
 </file>
@@ -163,10 +205,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -481,144 +524,312 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE53A7B4-A1CF-334B-A7B4-F41E4F3DE837}">
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="199" zoomScaleNormal="199" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="5" max="5" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="31.6640625" customWidth="1"/>
+    <col min="3" max="3" width="26.83203125" customWidth="1"/>
+    <col min="4" max="4" width="71.33203125" customWidth="1"/>
+    <col min="6" max="6" width="11.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E1" t="s">
+      <c r="B1" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5">
+        <v>24</v>
+      </c>
+      <c r="D5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="2"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7">
+        <v>28</v>
+      </c>
+      <c r="F7" s="2"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10">
+        <v>22</v>
+      </c>
+      <c r="D10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B11" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B13" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
+      <c r="B15" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
+      <c r="B16" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16">
+        <v>24</v>
+      </c>
+      <c r="D16" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
+      <c r="B17" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
+      <c r="B18" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
+      <c r="B19" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
+      <c r="B20" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C20" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
+      <c r="B21" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A22" s="1" t="s">
+      <c r="B22" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C22" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="s">
+      <c r="B23" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C23" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A24" s="1" t="s">
+      <c r="B24" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C24" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A25" s="1" t="s">
-        <v>24</v>
+      <c r="B25" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C25" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>